<commit_message>
EDIT -- Laporan dan Penerimaan barang
</commit_message>
<xml_diff>
--- a/public/tamplate pemesanan.xlsx
+++ b/public/tamplate pemesanan.xlsx
@@ -8,17 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/projek/tugas-rpl/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A86FF76-A3B8-0D44-BC49-35B850D1BF40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C860E4A4-D9EA-4540-9244-AE16CCAD7FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="15940" xr2:uid="{71F67EEA-BD1E-164C-9CF4-F727CD5E0FFB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AG$1129</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet1!$A$1:$AG$1129</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
+  <pivotCaches>
+    <pivotCache cacheId="2" r:id="rId4"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="132">
   <si>
     <t>Purchasing Document</t>
   </si>
@@ -427,6 +432,15 @@
   <si>
     <t>15-05-2025</t>
   </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Count of Material</t>
+  </si>
 </sst>
 </file>
 
@@ -476,7 +490,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -497,6 +511,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6844,6 +6863,1116 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="it rsup" refreshedDate="45864.79209988426" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="24" xr:uid="{A6036E9C-245A-C34C-8B6D-F13B3CEBF997}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:AG25" sheet="Sheet1"/>
+  </cacheSource>
+  <cacheFields count="33">
+    <cacheField name="Purchasing Document" numFmtId="0">
+      <sharedItems count="8">
+        <s v="4200025861"/>
+        <s v="4200025860"/>
+        <s v="4200025694"/>
+        <s v="4200025681"/>
+        <s v="4200025680"/>
+        <s v="4200025679"/>
+        <s v="4200025677"/>
+        <s v="4200025673"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Item" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Purchasing Doc. Type" numFmtId="49">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Release indicator" numFmtId="49">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Purchasing Group" numFmtId="49">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="PO history/release documentation" numFmtId="49">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Document Date" numFmtId="49">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Supplier/Supplying Plant" numFmtId="49">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Material" numFmtId="49">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Short Text" numFmtId="49">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Material Group" numFmtId="49">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Valuation Type" numFmtId="49">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Deletion Indicator" numFmtId="49">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Item Category" numFmtId="49">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Acct Assignment Cat." numFmtId="49">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Plant" numFmtId="49">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Storage location" numFmtId="49">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Order Quantity" numFmtId="49">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="18"/>
+    </cacheField>
+    <cacheField name="Order Unit" numFmtId="49">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Tax Code" numFmtId="49">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Quantity in SKU" numFmtId="49">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="18"/>
+    </cacheField>
+    <cacheField name="Stockkeeping unit" numFmtId="49">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Net Price" numFmtId="49">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="0"/>
+    </cacheField>
+    <cacheField name="Currency" numFmtId="49">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Price unit" numFmtId="49">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="8"/>
+    </cacheField>
+    <cacheField name="Still to be invoiced (val.)" numFmtId="49">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="0"/>
+    </cacheField>
+    <cacheField name="Still to be delivered (qty)" numFmtId="49">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="18"/>
+    </cacheField>
+    <cacheField name="Still to be delivered (value)" numFmtId="49">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="0"/>
+    </cacheField>
+    <cacheField name="Target Quantity" numFmtId="49">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="0"/>
+    </cacheField>
+    <cacheField name="Open Target Quantity" numFmtId="49">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="0"/>
+    </cacheField>
+    <cacheField name="Still to be invoiced (qty)" numFmtId="49">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="18"/>
+    </cacheField>
+    <cacheField name="No. of Positions" numFmtId="49">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="1"/>
+    </cacheField>
+    <cacheField name="Description" numFmtId="49">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="24">
+  <r>
+    <x v="0"/>
+    <s v="10"/>
+    <s v="ZOIM"/>
+    <s v="X"/>
+    <s v="D08"/>
+    <s v=""/>
+    <s v="28-05-2025"/>
+    <s v="10009824   SERAC ASIA SDN BHD"/>
+    <s v="70021052"/>
+    <s v="HEAT SEALING RESISTANCE,PNNV20603403C"/>
+    <s v="SPT40015"/>
+    <s v="Z-NEW"/>
+    <s v=""/>
+    <s v=""/>
+    <s v=""/>
+    <s v="2111"/>
+    <s v="SP01"/>
+    <n v="1"/>
+    <s v="PC"/>
+    <s v="I0"/>
+    <n v="1"/>
+    <s v="PC"/>
+    <n v="0"/>
+    <s v="EUR"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="10"/>
+    <s v="ZOIM"/>
+    <s v="X"/>
+    <s v="D08"/>
+    <s v=""/>
+    <s v="28-05-2025"/>
+    <s v="10472435   TEKNOICE SRL"/>
+    <s v="70028546"/>
+    <s v="CARTRIDGE RESISTOR,250W48V 6.5X70,C13440"/>
+    <s v="SPT40003"/>
+    <s v="Z-NEW"/>
+    <s v=""/>
+    <s v=""/>
+    <s v=""/>
+    <s v="2111"/>
+    <s v="SP01"/>
+    <n v="2"/>
+    <s v="PC"/>
+    <s v="I0"/>
+    <n v="2"/>
+    <s v="PC"/>
+    <n v="0"/>
+    <s v="EUR"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="2"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
+    <n v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="20"/>
+    <s v="ZOIM"/>
+    <s v="X"/>
+    <s v="D08"/>
+    <s v=""/>
+    <s v="28-05-2025"/>
+    <s v="10472435   TEKNOICE SRL"/>
+    <s v="70003137"/>
+    <s v="ROLL ROD GASKET,MW05020021"/>
+    <s v="SPT40003"/>
+    <s v="Z-NEW"/>
+    <s v=""/>
+    <s v=""/>
+    <s v=""/>
+    <s v="2111"/>
+    <s v="SP01"/>
+    <n v="10"/>
+    <s v="PC"/>
+    <s v="I0"/>
+    <n v="10"/>
+    <s v="PC"/>
+    <n v="0"/>
+    <s v="EUR"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="10"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="10"/>
+    <n v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="30"/>
+    <s v="ZOIM"/>
+    <s v="X"/>
+    <s v="D08"/>
+    <s v=""/>
+    <s v="28-05-2025"/>
+    <s v="10472435   TEKNOICE SRL"/>
+    <s v="70028396"/>
+    <s v="THERMOCOUPLE,PT100 4X30WIRE1MT,C02861"/>
+    <s v="SPT40003"/>
+    <s v="Z-NEW"/>
+    <s v=""/>
+    <s v=""/>
+    <s v=""/>
+    <s v="2111"/>
+    <s v="SP01"/>
+    <n v="1"/>
+    <s v="PC"/>
+    <s v="I0"/>
+    <n v="1"/>
+    <s v="PC"/>
+    <n v="0"/>
+    <s v="EUR"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="10"/>
+    <s v="ZOIM"/>
+    <s v="R"/>
+    <s v="D08"/>
+    <s v=""/>
+    <s v="19-05-2025"/>
+    <s v="10557169   MESPACK SL"/>
+    <s v="70034345"/>
+    <s v="FRONT SEALER COVER,33.09.7.01.14.1"/>
+    <s v="SPT40083"/>
+    <s v="Z-NEW"/>
+    <s v=""/>
+    <s v=""/>
+    <s v=""/>
+    <s v="2111"/>
+    <s v="SP01"/>
+    <n v="6"/>
+    <s v="PC"/>
+    <s v="I0"/>
+    <n v="6"/>
+    <s v="PC"/>
+    <n v="0"/>
+    <s v="EUR"/>
+    <n v="6"/>
+    <n v="0"/>
+    <n v="6"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="6"/>
+    <n v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="20"/>
+    <s v="ZOIM"/>
+    <s v="R"/>
+    <s v="D08"/>
+    <s v=""/>
+    <s v="19-05-2025"/>
+    <s v="10557169   MESPACK SL"/>
+    <s v="70034346"/>
+    <s v="REAR WELDER PROTECTION,36.09.6.05.02.0"/>
+    <s v="SPT40083"/>
+    <s v="Z-NEW"/>
+    <s v=""/>
+    <s v=""/>
+    <s v=""/>
+    <s v="2111"/>
+    <s v="SP01"/>
+    <n v="2"/>
+    <s v="PC"/>
+    <s v="I0"/>
+    <n v="2"/>
+    <s v="PC"/>
+    <n v="0"/>
+    <s v="EUR"/>
+    <n v="2"/>
+    <n v="0"/>
+    <n v="2"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
+    <n v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="30"/>
+    <s v="ZOIM"/>
+    <s v="R"/>
+    <s v="D08"/>
+    <s v=""/>
+    <s v="19-05-2025"/>
+    <s v="10557169   MESPACK SL"/>
+    <s v="70034335"/>
+    <s v="FRONT SEALER COVER,36.09.7.02.04.0"/>
+    <s v="SPT40083"/>
+    <s v="Z-NEW"/>
+    <s v=""/>
+    <s v=""/>
+    <s v=""/>
+    <s v="2111"/>
+    <s v="SP01"/>
+    <n v="8"/>
+    <s v="PC"/>
+    <s v="I0"/>
+    <n v="8"/>
+    <s v="PC"/>
+    <n v="0"/>
+    <s v="EUR"/>
+    <n v="8"/>
+    <n v="0"/>
+    <n v="8"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="8"/>
+    <n v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="40"/>
+    <s v="ZOIM"/>
+    <s v="R"/>
+    <s v="D08"/>
+    <s v=""/>
+    <s v="19-05-2025"/>
+    <s v="10557169   MESPACK SL"/>
+    <s v="70034367"/>
+    <s v="REAR ISOLATOR,36.09.7.01.02.0"/>
+    <s v="SPT40083"/>
+    <s v="Z-NEW"/>
+    <s v=""/>
+    <s v=""/>
+    <s v=""/>
+    <s v="2111"/>
+    <s v="SP01"/>
+    <n v="1"/>
+    <s v="PC"/>
+    <s v="I0"/>
+    <n v="1"/>
+    <s v="PC"/>
+    <n v="0"/>
+    <s v="EUR"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="50"/>
+    <s v="ZOIM"/>
+    <s v="R"/>
+    <s v="D08"/>
+    <s v=""/>
+    <s v="19-05-2025"/>
+    <s v="10557169   MESPACK SL"/>
+    <s v="70034337"/>
+    <s v="REAR WELDER PROTECTION,36.09.6.06.02.0"/>
+    <s v="SPT40083"/>
+    <s v="Z-NEW"/>
+    <s v=""/>
+    <s v=""/>
+    <s v=""/>
+    <s v="2111"/>
+    <s v="SP01"/>
+    <n v="2"/>
+    <s v="PC"/>
+    <s v="I0"/>
+    <n v="2"/>
+    <s v="PC"/>
+    <n v="0"/>
+    <s v="EUR"/>
+    <n v="2"/>
+    <n v="0"/>
+    <n v="2"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
+    <n v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="60"/>
+    <s v="ZOIM"/>
+    <s v="R"/>
+    <s v="D08"/>
+    <s v=""/>
+    <s v="19-05-2025"/>
+    <s v="10557169   MESPACK SL"/>
+    <s v="70034360"/>
+    <s v="COOLER SILICONE,540.29.0.01.01.0"/>
+    <s v="SPT40083"/>
+    <s v="Z-NEW"/>
+    <s v=""/>
+    <s v=""/>
+    <s v=""/>
+    <s v="2111"/>
+    <s v="SP01"/>
+    <n v="8"/>
+    <s v="PC"/>
+    <s v="I0"/>
+    <n v="8"/>
+    <s v="PC"/>
+    <n v="0"/>
+    <s v="EUR"/>
+    <n v="8"/>
+    <n v="0"/>
+    <n v="8"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="8"/>
+    <n v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="70"/>
+    <s v="ZOIM"/>
+    <s v="R"/>
+    <s v="D08"/>
+    <s v=""/>
+    <s v="19-05-2025"/>
+    <s v="10557169   MESPACK SL"/>
+    <s v="70034364"/>
+    <s v="REAR COOLER SILICON,36.29.6.12.01.0"/>
+    <s v="SPT40083"/>
+    <s v="Z-NEW"/>
+    <s v=""/>
+    <s v=""/>
+    <s v=""/>
+    <s v="2111"/>
+    <s v="SP01"/>
+    <n v="4"/>
+    <s v="PC"/>
+    <s v="I0"/>
+    <n v="4"/>
+    <s v="PC"/>
+    <n v="0"/>
+    <s v="EUR"/>
+    <n v="4"/>
+    <n v="0"/>
+    <n v="4"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="4"/>
+    <n v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="80"/>
+    <s v="ZOIM"/>
+    <s v="R"/>
+    <s v="D08"/>
+    <s v=""/>
+    <s v="19-05-2025"/>
+    <s v="10557169   MESPACK SL"/>
+    <s v="70033223"/>
+    <s v="SUPPORT CYLINDER,PNCN0101848B"/>
+    <s v="SPT40083"/>
+    <s v="Z-NEW"/>
+    <s v=""/>
+    <s v=""/>
+    <s v=""/>
+    <s v="2111"/>
+    <s v="SP01"/>
+    <n v="4"/>
+    <s v="PC"/>
+    <s v="I0"/>
+    <n v="4"/>
+    <s v="PC"/>
+    <n v="0"/>
+    <s v="EUR"/>
+    <n v="4"/>
+    <n v="0"/>
+    <n v="4"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="4"/>
+    <n v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="10"/>
+    <s v="ZOIM"/>
+    <s v="R"/>
+    <s v="D08"/>
+    <s v=""/>
+    <s v="16-05-2025"/>
+    <s v="10470307   EVERGREEN PACKAGING LLC"/>
+    <s v="70002273"/>
+    <s v="BRUSHES MOTOR (SET OF 2),PNEP5904486"/>
+    <s v="SPT40005"/>
+    <s v="Z-NEW"/>
+    <s v=""/>
+    <s v=""/>
+    <s v=""/>
+    <s v="2111"/>
+    <s v="SP01"/>
+    <n v="8"/>
+    <s v="PC"/>
+    <s v="I0"/>
+    <n v="8"/>
+    <s v="PC"/>
+    <n v="0"/>
+    <s v="USD"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="8"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="8"/>
+    <n v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="10"/>
+    <s v="ZOIM"/>
+    <s v="R"/>
+    <s v="D08"/>
+    <s v=""/>
+    <s v="16-05-2025"/>
+    <s v="10603548   FBR ELPO SPA"/>
+    <s v="70034448"/>
+    <s v="VALVE,DN50XDN50,D47-309"/>
+    <s v="SPT40060"/>
+    <s v="Z-NEW"/>
+    <s v=""/>
+    <s v=""/>
+    <s v=""/>
+    <s v="2111"/>
+    <s v="SP01"/>
+    <n v="2"/>
+    <s v="PC"/>
+    <s v="I0"/>
+    <n v="2"/>
+    <s v="PC"/>
+    <n v="0"/>
+    <s v="EUR"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="2"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2"/>
+    <n v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="10"/>
+    <s v="ZOIM"/>
+    <s v="R"/>
+    <s v="D08"/>
+    <s v=""/>
+    <s v="16-05-2025"/>
+    <s v="10009445   GRAM EQUIPMENT A/S"/>
+    <s v="70006394"/>
+    <s v="&quot;SCRAPER BLADE W/O HOLES,PN78162208113&quot;"/>
+    <s v="SPT40002"/>
+    <s v="Z-NEW"/>
+    <s v=""/>
+    <s v=""/>
+    <s v=""/>
+    <s v="2111"/>
+    <s v="SP01"/>
+    <n v="18"/>
+    <s v="PC"/>
+    <s v="I0"/>
+    <n v="18"/>
+    <s v="PC"/>
+    <n v="0"/>
+    <s v="EUR"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="18"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="18"/>
+    <n v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="6"/>
+    <s v="10"/>
+    <s v="ZOIM"/>
+    <s v="R"/>
+    <s v="D08"/>
+    <s v=""/>
+    <s v="16-05-2025"/>
+    <s v="10645494   DSI DANTECH AAL A/S"/>
+    <s v="70034394"/>
+    <s v="DRUM CHAIN,PI080014"/>
+    <s v="SPT40019"/>
+    <s v="Z-NEW"/>
+    <s v=""/>
+    <s v=""/>
+    <s v=""/>
+    <s v="2111"/>
+    <s v="SP01"/>
+    <n v="10"/>
+    <s v="M"/>
+    <s v="I0"/>
+    <n v="10"/>
+    <s v="M"/>
+    <n v="0"/>
+    <s v="EUR"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="10"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="10"/>
+    <n v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="6"/>
+    <s v="20"/>
+    <s v="ZOIM"/>
+    <s v="R"/>
+    <s v="D08"/>
+    <m/>
+    <s v="16-05-2025"/>
+    <s v="10645494   DSI DANTECH AAL A/S"/>
+    <s v="70034395"/>
+    <s v="OFFSET LINK,PI080069"/>
+    <s v="SPT40019"/>
+    <s v="Z-NEW"/>
+    <s v=""/>
+    <s v=""/>
+    <s v=""/>
+    <s v="2111"/>
+    <s v="SP01"/>
+    <n v="1"/>
+    <s v="PC"/>
+    <s v="I0"/>
+    <n v="1"/>
+    <s v="PC"/>
+    <n v="0"/>
+    <s v="EUR"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="7"/>
+    <s v="10"/>
+    <s v="ZOIM"/>
+    <s v="R"/>
+    <s v="D08"/>
+    <s v=""/>
+    <s v="15-05-2025"/>
+    <s v="10645494   DSI DANTECH AAL A/S"/>
+    <s v="70034393"/>
+    <s v="EVAPORATOR FAN IMPELLER,SPARE002"/>
+    <s v="SPT40019"/>
+    <s v="Z-NEW"/>
+    <s v=""/>
+    <s v=""/>
+    <s v=""/>
+    <s v="2111"/>
+    <s v="SP01"/>
+    <n v="1"/>
+    <s v="PC"/>
+    <s v="I0"/>
+    <n v="1"/>
+    <s v="PC"/>
+    <n v="0"/>
+    <s v="EUR"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="7"/>
+    <s v="20"/>
+    <s v="ZOIM"/>
+    <s v="R"/>
+    <s v="D08"/>
+    <s v=""/>
+    <s v="15-05-2025"/>
+    <s v="10645494   DSI DANTECH AAL A/S"/>
+    <s v="70034396"/>
+    <s v="DRUM MOTOR SPROCKET,GALVANIZED,PI120002"/>
+    <s v="SPT40019"/>
+    <s v="Z-NEW"/>
+    <s v=""/>
+    <s v=""/>
+    <s v=""/>
+    <s v="2111"/>
+    <s v="SP01"/>
+    <n v="1"/>
+    <s v="PC"/>
+    <s v="I0"/>
+    <n v="1"/>
+    <s v="PC"/>
+    <n v="0"/>
+    <s v="EUR"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="7"/>
+    <s v="30"/>
+    <s v="ZOIM"/>
+    <s v="R"/>
+    <s v="D08"/>
+    <s v=""/>
+    <s v="15-05-2025"/>
+    <s v="10645494   DSI DANTECH AAL A/S"/>
+    <s v="70034398"/>
+    <s v="DRUM CHAIN SPROCKET,SPARE001"/>
+    <s v="SPT40019"/>
+    <s v="Z-NEW"/>
+    <s v=""/>
+    <s v=""/>
+    <s v=""/>
+    <s v="2111"/>
+    <s v="SP01"/>
+    <n v="1"/>
+    <s v="SET"/>
+    <s v="I0"/>
+    <n v="1"/>
+    <s v="SET"/>
+    <n v="0"/>
+    <s v="EUR"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="7"/>
+    <s v="40"/>
+    <s v="ZOIM"/>
+    <s v="R"/>
+    <s v="D08"/>
+    <s v=""/>
+    <s v="15-05-2025"/>
+    <s v="10645494   DSI DANTECH AAL A/S"/>
+    <s v="70034399"/>
+    <s v="BOTTOM BEARING,60X130X46MM,PA000032"/>
+    <s v="SPT40019"/>
+    <s v="Z-NEW"/>
+    <s v=""/>
+    <s v=""/>
+    <s v=""/>
+    <s v="2111"/>
+    <s v="SP01"/>
+    <n v="1"/>
+    <s v="PC"/>
+    <s v="I0"/>
+    <n v="1"/>
+    <s v="PC"/>
+    <n v="0"/>
+    <s v="EUR"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="7"/>
+    <s v="50"/>
+    <s v="ZOIM"/>
+    <s v="R"/>
+    <s v="D08"/>
+    <s v=""/>
+    <s v="15-05-2025"/>
+    <s v="10645494   DSI DANTECH AAL A/S"/>
+    <s v="70034400"/>
+    <s v="OIL SEAL FOR BOTTOM BEARING,PA000022"/>
+    <s v="SPT40019"/>
+    <s v="Z-NEW"/>
+    <s v=""/>
+    <s v=""/>
+    <s v=""/>
+    <s v="2111"/>
+    <s v="SP01"/>
+    <n v="1"/>
+    <s v="PC"/>
+    <s v="I0"/>
+    <n v="1"/>
+    <s v="PC"/>
+    <n v="0"/>
+    <s v="EUR"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="7"/>
+    <s v="60"/>
+    <s v="ZOIM"/>
+    <s v="R"/>
+    <s v="D08"/>
+    <s v=""/>
+    <s v="15-05-2025"/>
+    <s v="10645494   DSI DANTECH AAL A/S"/>
+    <s v="70034401"/>
+    <s v="INVERTER,1.5KW,PC190149-1"/>
+    <s v="SPT40019"/>
+    <s v="Z-NEW"/>
+    <s v=""/>
+    <s v=""/>
+    <s v=""/>
+    <s v="2111"/>
+    <s v="SP01"/>
+    <n v="1"/>
+    <s v="PC"/>
+    <s v="I0"/>
+    <n v="1"/>
+    <s v="PC"/>
+    <n v="0"/>
+    <s v="EUR"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="7"/>
+    <s v="70"/>
+    <s v="ZOIM"/>
+    <s v="R"/>
+    <s v="D08"/>
+    <s v=""/>
+    <s v="15-05-2025"/>
+    <s v="10645494   DSI DANTECH AAL A/S"/>
+    <s v="70034402"/>
+    <s v="VLT CONTROL PANEL LCP 21,PC190159"/>
+    <s v="SPT40019"/>
+    <s v="Z-NEW"/>
+    <s v=""/>
+    <s v=""/>
+    <s v=""/>
+    <s v="2111"/>
+    <s v="SP01"/>
+    <n v="1"/>
+    <s v="PC"/>
+    <s v="I0"/>
+    <n v="1"/>
+    <s v="PC"/>
+    <n v="0"/>
+    <s v="EUR"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <m/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DE1F426F-55F6-3144-827D-DA42EF489602}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="33">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="9">
+        <item x="7"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="49" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="49" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="49" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="49" showAll="0"/>
+    <pivotField numFmtId="49" showAll="0"/>
+    <pivotField numFmtId="49" showAll="0"/>
+    <pivotField numFmtId="49" showAll="0"/>
+    <pivotField numFmtId="49" showAll="0"/>
+    <pivotField numFmtId="49" showAll="0"/>
+    <pivotField numFmtId="49" showAll="0"/>
+    <pivotField numFmtId="49" showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Material" fld="8" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{704EC647-537C-E341-9DCE-BD4FF922C1E8}" name="Table1" displayName="Table1" ref="A1:AG8" totalsRowShown="0">
+  <autoFilter ref="A1:AG8" xr:uid="{704EC647-537C-E341-9DCE-BD4FF922C1E8}"/>
+  <tableColumns count="33">
+    <tableColumn id="1" xr3:uid="{000CBEBD-91BE-0C40-93A8-E7DCEB826291}" name="Purchasing Document"/>
+    <tableColumn id="2" xr3:uid="{868721ED-43F5-394F-94C8-63AEE3DF40B6}" name="Item"/>
+    <tableColumn id="3" xr3:uid="{4C09B81F-1B2D-C043-9F0F-8204E6306037}" name="Purchasing Doc. Type"/>
+    <tableColumn id="4" xr3:uid="{AFF650AC-A510-694B-ADD0-484A1AC19A3A}" name="Release indicator"/>
+    <tableColumn id="5" xr3:uid="{E925C957-067E-6547-9211-FD57D8761263}" name="Purchasing Group"/>
+    <tableColumn id="6" xr3:uid="{9122E956-FA0B-D946-AB66-68351B7DC1B0}" name="PO history/release documentation"/>
+    <tableColumn id="7" xr3:uid="{D67DBB33-5917-CF4E-9BB2-E1E147B45071}" name="Document Date"/>
+    <tableColumn id="8" xr3:uid="{660A5D46-5D9C-F14E-813E-751E92A6C05B}" name="Supplier/Supplying Plant"/>
+    <tableColumn id="9" xr3:uid="{74EA023F-9E1D-3A49-8CEC-754F70CC0DE8}" name="Material"/>
+    <tableColumn id="10" xr3:uid="{7933C6DC-99B5-2740-AB39-FF85C6B2499B}" name="Short Text"/>
+    <tableColumn id="11" xr3:uid="{3BDEF73D-5F2C-4440-A492-CAB68B4CA5F7}" name="Material Group"/>
+    <tableColumn id="12" xr3:uid="{F1307C9F-BD6E-344B-91DC-34BFE6D77871}" name="Valuation Type"/>
+    <tableColumn id="13" xr3:uid="{DDFE4CC0-7CD9-F241-A651-474DABBBBDD8}" name="Deletion Indicator"/>
+    <tableColumn id="14" xr3:uid="{7DA8E89F-482C-C54A-95B9-4F662AF82BE1}" name="Item Category"/>
+    <tableColumn id="15" xr3:uid="{F043798A-2B4F-D840-BA6B-250F92C40145}" name="Acct Assignment Cat."/>
+    <tableColumn id="16" xr3:uid="{0DE6B186-0029-5949-8164-A1D2605EA945}" name="Plant"/>
+    <tableColumn id="17" xr3:uid="{EA0CA749-EE1E-2D4F-86C8-5ED764CA09D3}" name="Storage location"/>
+    <tableColumn id="18" xr3:uid="{A22F484F-05EA-1F45-8578-8D9B11B9A6D8}" name="Order Quantity"/>
+    <tableColumn id="19" xr3:uid="{4B648069-0F07-034F-838A-F608ACB8C80F}" name="Order Unit"/>
+    <tableColumn id="20" xr3:uid="{54880DD0-B034-9146-B561-89D0430F8FFD}" name="Tax Code"/>
+    <tableColumn id="21" xr3:uid="{40A8269F-A881-D44D-8F88-F57FAE4A94AC}" name="Quantity in SKU"/>
+    <tableColumn id="22" xr3:uid="{140C563E-F4F3-B24D-95B9-E25AC6B22D04}" name="Stockkeeping unit"/>
+    <tableColumn id="23" xr3:uid="{35E2DC56-8D49-EF43-840B-4B8563967AAF}" name="Net Price"/>
+    <tableColumn id="24" xr3:uid="{A7AB681A-58A2-EF47-B4B2-78F0A2726ECB}" name="Currency"/>
+    <tableColumn id="25" xr3:uid="{143809B9-2565-984A-87AE-9D52F169B201}" name="Price unit"/>
+    <tableColumn id="26" xr3:uid="{FE20576E-0B15-4B4F-95BB-80124C5D7B5A}" name="Still to be invoiced (val.)"/>
+    <tableColumn id="27" xr3:uid="{B5FF2956-5B5F-E949-BEBC-140FD814D345}" name="Still to be delivered (qty)"/>
+    <tableColumn id="28" xr3:uid="{0BE7485F-8A69-954E-A84C-27860B7DBCFF}" name="Still to be delivered (value)"/>
+    <tableColumn id="29" xr3:uid="{9E378429-2400-8040-A02E-E4BAD18266A9}" name="Target Quantity"/>
+    <tableColumn id="30" xr3:uid="{84BB0424-85C8-CA46-8741-1550709D7442}" name="Open Target Quantity"/>
+    <tableColumn id="31" xr3:uid="{4BC226EB-BBAA-4F45-B30E-3D1297618384}" name="Still to be invoiced (qty)"/>
+    <tableColumn id="32" xr3:uid="{35B3EE65-9D4F-FE4F-B413-802588DA3E33}" name="No. of Positions"/>
+    <tableColumn id="33" xr3:uid="{59633F38-A4A0-FD4E-B098-9564BE6BA95F}" name="Description"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -7160,11 +8289,946 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCB4E616-FB68-794F-8296-EC3023599189}">
+  <dimension ref="A1:AG8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" customWidth="1"/>
+    <col min="6" max="6" width="31.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.5" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" customWidth="1"/>
+    <col min="10" max="10" width="11.5" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" customWidth="1"/>
+    <col min="13" max="13" width="18.1640625" customWidth="1"/>
+    <col min="14" max="14" width="15.1640625" customWidth="1"/>
+    <col min="15" max="15" width="21.5" customWidth="1"/>
+    <col min="17" max="17" width="16.83203125" customWidth="1"/>
+    <col min="18" max="18" width="15.5" customWidth="1"/>
+    <col min="19" max="19" width="11.83203125" customWidth="1"/>
+    <col min="21" max="21" width="16" customWidth="1"/>
+    <col min="22" max="22" width="18.1640625" customWidth="1"/>
+    <col min="23" max="23" width="11.1640625" customWidth="1"/>
+    <col min="24" max="24" width="11" customWidth="1"/>
+    <col min="25" max="25" width="11.33203125" customWidth="1"/>
+    <col min="26" max="26" width="22.6640625" customWidth="1"/>
+    <col min="27" max="27" width="23" customWidth="1"/>
+    <col min="28" max="28" width="24.83203125" customWidth="1"/>
+    <col min="29" max="29" width="16" customWidth="1"/>
+    <col min="30" max="30" width="20.6640625" customWidth="1"/>
+    <col min="31" max="31" width="22.33203125" customWidth="1"/>
+    <col min="32" max="32" width="16.5" customWidth="1"/>
+    <col min="33" max="33" width="13.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I2" t="s">
+        <v>123</v>
+      </c>
+      <c r="J2" t="s">
+        <v>124</v>
+      </c>
+      <c r="K2" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P2" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>45</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2" t="s">
+        <v>46</v>
+      </c>
+      <c r="T2" t="s">
+        <v>47</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2" t="s">
+        <v>46</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y2">
+        <v>1</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>1</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>1</v>
+      </c>
+      <c r="AF2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" t="s">
+        <v>128</v>
+      </c>
+      <c r="H3" t="s">
+        <v>102</v>
+      </c>
+      <c r="I3" t="s">
+        <v>121</v>
+      </c>
+      <c r="J3" t="s">
+        <v>122</v>
+      </c>
+      <c r="K3" t="s">
+        <v>105</v>
+      </c>
+      <c r="L3" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N3" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>45</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3" t="s">
+        <v>46</v>
+      </c>
+      <c r="T3" t="s">
+        <v>47</v>
+      </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3" t="s">
+        <v>46</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y3">
+        <v>1</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>1</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>1</v>
+      </c>
+      <c r="AF3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" t="s">
+        <v>128</v>
+      </c>
+      <c r="H4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I4" t="s">
+        <v>119</v>
+      </c>
+      <c r="J4" t="s">
+        <v>120</v>
+      </c>
+      <c r="K4" t="s">
+        <v>105</v>
+      </c>
+      <c r="L4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M4" t="s">
+        <v>38</v>
+      </c>
+      <c r="N4" t="s">
+        <v>38</v>
+      </c>
+      <c r="O4" t="s">
+        <v>38</v>
+      </c>
+      <c r="P4" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>45</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4" t="s">
+        <v>46</v>
+      </c>
+      <c r="T4" t="s">
+        <v>47</v>
+      </c>
+      <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4" t="s">
+        <v>46</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y4">
+        <v>1</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>1</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>1</v>
+      </c>
+      <c r="AF4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" t="s">
+        <v>128</v>
+      </c>
+      <c r="H5" t="s">
+        <v>102</v>
+      </c>
+      <c r="I5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J5" t="s">
+        <v>118</v>
+      </c>
+      <c r="K5" t="s">
+        <v>105</v>
+      </c>
+      <c r="L5" t="s">
+        <v>43</v>
+      </c>
+      <c r="M5" t="s">
+        <v>38</v>
+      </c>
+      <c r="N5" t="s">
+        <v>38</v>
+      </c>
+      <c r="O5" t="s">
+        <v>38</v>
+      </c>
+      <c r="P5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>45</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5" t="s">
+        <v>46</v>
+      </c>
+      <c r="T5" t="s">
+        <v>47</v>
+      </c>
+      <c r="U5">
+        <v>1</v>
+      </c>
+      <c r="V5" t="s">
+        <v>46</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y5">
+        <v>1</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>1</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>1</v>
+      </c>
+      <c r="AF5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" t="s">
+        <v>128</v>
+      </c>
+      <c r="H6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I6" t="s">
+        <v>114</v>
+      </c>
+      <c r="J6" t="s">
+        <v>115</v>
+      </c>
+      <c r="K6" t="s">
+        <v>105</v>
+      </c>
+      <c r="L6" t="s">
+        <v>43</v>
+      </c>
+      <c r="M6" t="s">
+        <v>38</v>
+      </c>
+      <c r="N6" t="s">
+        <v>38</v>
+      </c>
+      <c r="O6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P6" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>45</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6" t="s">
+        <v>116</v>
+      </c>
+      <c r="T6" t="s">
+        <v>47</v>
+      </c>
+      <c r="U6">
+        <v>1</v>
+      </c>
+      <c r="V6" t="s">
+        <v>116</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y6">
+        <v>1</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <v>1</v>
+      </c>
+      <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <v>0</v>
+      </c>
+      <c r="AE6">
+        <v>1</v>
+      </c>
+      <c r="AF6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" t="s">
+        <v>128</v>
+      </c>
+      <c r="H7" t="s">
+        <v>102</v>
+      </c>
+      <c r="I7" t="s">
+        <v>112</v>
+      </c>
+      <c r="J7" t="s">
+        <v>113</v>
+      </c>
+      <c r="K7" t="s">
+        <v>105</v>
+      </c>
+      <c r="L7" t="s">
+        <v>43</v>
+      </c>
+      <c r="M7" t="s">
+        <v>38</v>
+      </c>
+      <c r="N7" t="s">
+        <v>38</v>
+      </c>
+      <c r="O7" t="s">
+        <v>38</v>
+      </c>
+      <c r="P7" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>45</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7" t="s">
+        <v>46</v>
+      </c>
+      <c r="T7" t="s">
+        <v>47</v>
+      </c>
+      <c r="U7">
+        <v>1</v>
+      </c>
+      <c r="V7" t="s">
+        <v>46</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y7">
+        <v>1</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <v>1</v>
+      </c>
+      <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+      <c r="AE7">
+        <v>1</v>
+      </c>
+      <c r="AF7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" t="s">
+        <v>128</v>
+      </c>
+      <c r="H8" t="s">
+        <v>102</v>
+      </c>
+      <c r="I8" t="s">
+        <v>110</v>
+      </c>
+      <c r="J8" t="s">
+        <v>111</v>
+      </c>
+      <c r="K8" t="s">
+        <v>105</v>
+      </c>
+      <c r="L8" t="s">
+        <v>43</v>
+      </c>
+      <c r="M8" t="s">
+        <v>38</v>
+      </c>
+      <c r="N8" t="s">
+        <v>38</v>
+      </c>
+      <c r="O8" t="s">
+        <v>38</v>
+      </c>
+      <c r="P8" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>45</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8" t="s">
+        <v>46</v>
+      </c>
+      <c r="T8" t="s">
+        <v>47</v>
+      </c>
+      <c r="U8">
+        <v>1</v>
+      </c>
+      <c r="V8" t="s">
+        <v>46</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y8">
+        <v>1</v>
+      </c>
+      <c r="Z8">
+        <v>0</v>
+      </c>
+      <c r="AA8">
+        <v>1</v>
+      </c>
+      <c r="AB8">
+        <v>0</v>
+      </c>
+      <c r="AC8">
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <v>0</v>
+      </c>
+      <c r="AE8">
+        <v>1</v>
+      </c>
+      <c r="AF8">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB68632-8D52-9C4F-82B9-CE05B3B18EAF}">
+  <dimension ref="A3:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B12" s="10">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76EAD5CA-EAA3-834B-9E94-188060D9B609}">
   <dimension ref="A1:AG1129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
EDIT -- Pemesanan Import dibuatt langsung tambah barang ketika barangnya tidak ditemukan
</commit_message>
<xml_diff>
--- a/public/tamplate pemesanan.xlsx
+++ b/public/tamplate pemesanan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/projek/tugas-rpl/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C860E4A4-D9EA-4540-9244-AE16CCAD7FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B661576C-45DD-4E4F-825E-EC49C4B5A450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="15940" xr2:uid="{71F67EEA-BD1E-164C-9CF4-F727CD5E0FFB}"/>
+    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="15940" activeTab="2" xr2:uid="{71F67EEA-BD1E-164C-9CF4-F727CD5E0FFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId4"/>
+    <pivotCache cacheId="3" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="134">
   <si>
     <t>Purchasing Document</t>
   </si>
@@ -441,6 +441,12 @@
   <si>
     <t>Count of Material</t>
   </si>
+  <si>
+    <t>06022005</t>
+  </si>
+  <si>
+    <t>Barangku</t>
+  </si>
 </sst>
 </file>
 
@@ -490,7 +496,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -515,7 +521,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7832,7 +7837,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DE1F426F-55F6-3144-827D-DA42EF489602}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DE1F426F-55F6-3144-827D-DA42EF489602}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="33">
     <pivotField axis="axisRow" showAll="0">
@@ -8292,8 +8297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCB4E616-FB68-794F-8296-EC3023599189}">
   <dimension ref="A1:AG8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9150,7 +9155,7 @@
       <c r="A4" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4">
         <v>7</v>
       </c>
     </row>
@@ -9158,7 +9163,7 @@
       <c r="A5" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5">
         <v>2</v>
       </c>
     </row>
@@ -9166,7 +9171,7 @@
       <c r="A6" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6">
         <v>1</v>
       </c>
     </row>
@@ -9174,7 +9179,7 @@
       <c r="A7" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7">
         <v>1</v>
       </c>
     </row>
@@ -9182,7 +9187,7 @@
       <c r="A8" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8">
         <v>1</v>
       </c>
     </row>
@@ -9190,7 +9195,7 @@
       <c r="A9" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9">
         <v>8</v>
       </c>
     </row>
@@ -9198,7 +9203,7 @@
       <c r="A10" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10">
         <v>3</v>
       </c>
     </row>
@@ -9206,7 +9211,7 @@
       <c r="A11" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11">
         <v>1</v>
       </c>
     </row>
@@ -9214,7 +9219,7 @@
       <c r="A12" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12">
         <v>24</v>
       </c>
     </row>
@@ -9227,8 +9232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76EAD5CA-EAA3-834B-9E94-188060D9B609}">
   <dimension ref="A1:AG1129"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11718,38 +11723,102 @@
       </c>
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
-      <c r="R26" s="5"/>
-      <c r="S26" s="4"/>
-      <c r="T26" s="4"/>
-      <c r="U26" s="5"/>
-      <c r="V26" s="4"/>
-      <c r="W26" s="5"/>
-      <c r="X26" s="4"/>
-      <c r="Y26" s="5"/>
-      <c r="Z26" s="5"/>
-      <c r="AA26" s="5"/>
-      <c r="AB26" s="5"/>
-      <c r="AC26" s="5"/>
-      <c r="AD26" s="5"/>
-      <c r="AE26" s="5"/>
-      <c r="AF26" s="5"/>
+      <c r="A26" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M26" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="N26" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="O26" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="P26" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q26" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="R26" s="5">
+        <v>1</v>
+      </c>
+      <c r="S26" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="T26" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="U26" s="5">
+        <v>1</v>
+      </c>
+      <c r="V26" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="W26" s="5">
+        <v>0</v>
+      </c>
+      <c r="X26" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y26" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z26" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA26" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB26" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC26" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD26" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE26" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF26" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>

</xml_diff>